<commit_message>
successful test writing single-feature project line to table FC in desktop
</commit_message>
<xml_diff>
--- a/gp-services/GP_Publishing_SOP.xlsx
+++ b/gp-services/GP_Publishing_SOP.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA3\gp-services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BBFDC9-BD8F-46B0-8625-973B67311366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1126A4-7ABB-4D37-901E-3AB6EE91A7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Publish Script" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1105,7 +1105,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>